<commit_message>
Whole series of small changes, lots of working with zigzag data
</commit_message>
<xml_diff>
--- a/summary_densitydata.xlsx
+++ b/summary_densitydata.xlsx
@@ -12,20 +12,80 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>SWE1</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SWE2</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>SWE3</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>SWE4</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>SWE5</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>SWE6</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>SWE7</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>SWE8</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>SWE9</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>elev</t>
+  </si>
+  <si>
+    <t>G04_Z3A_SWE</t>
+  </si>
+  <si>
     <t>density</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>G02_LSP</t>
   </si>
   <si>
@@ -50,72 +110,12 @@
     <t>G13_LSP</t>
   </si>
   <si>
-    <t>SWE1</t>
-  </si>
-  <si>
     <t>G13_USP</t>
   </si>
   <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SWE2</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>SWE3</t>
-  </si>
-  <si>
     <t>G13_ASP</t>
   </si>
   <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>SWE4</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>SWE5</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>SWE6</t>
-  </si>
-  <si>
-    <t>Q6</t>
-  </si>
-  <si>
-    <t>SWE7</t>
-  </si>
-  <si>
-    <t>Q7</t>
-  </si>
-  <si>
-    <t>SWE8</t>
-  </si>
-  <si>
-    <t>Q8</t>
-  </si>
-  <si>
-    <t>SWE9</t>
-  </si>
-  <si>
-    <t>Q9</t>
-  </si>
-  <si>
-    <t>elev</t>
-  </si>
-  <si>
-    <t>G04_Z3A_SWE</t>
-  </si>
-  <si>
     <t>G04_Z2A_SWE</t>
   </si>
   <si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>G02_Z7C_SWE</t>
+  </si>
+  <si>
+    <t>G03_Z3B_SWE</t>
   </si>
   <si>
     <t>GL13_ASP</t>
@@ -256,15 +259,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
@@ -272,7 +269,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -294,6 +297,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
@@ -324,156 +339,156 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="5">
         <v>362.84</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>598830.956872462</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="5">
         <v>6755272.76759921</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="5">
         <v>400.0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>599197.57</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="5">
         <v>6754686.13</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5">
         <v>323.36</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>600044.719257886</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <v>6754368.04943599</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="5">
         <v>298.8235294118</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>601779.320498905</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <v>6753115.5549246</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="5">
         <v>298.82</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="5">
         <v>596454.888567045</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="5">
         <v>6739984.58756568</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="5">
         <v>322.26</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="5">
         <v>595510.630882847</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="5">
         <v>6740736.35252594</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="5">
         <v>368.26</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="5">
         <v>595126.583444399</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="5">
         <v>6742232.89922962</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="5">
         <v>358.0</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="5">
         <v>603270.56558006</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="5">
         <v>6764638.61521979</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="5">
         <v>355.7</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="5">
         <v>604509.073083514</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="5">
         <v>6763342.34093057</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="5">
         <v>303.46</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="5">
         <v>606342.040716066</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="5">
         <v>6761736.67808849</v>
       </c>
     </row>
@@ -511,84 +526,84 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="3" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>321.05</v>
       </c>
       <c r="C2" s="6">
         <v>0.0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>321.24</v>
       </c>
       <c r="E2" s="6">
@@ -625,8 +640,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
+      <c r="A3" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B3" s="8">
         <v>322.98</v>
@@ -634,7 +649,7 @@
       <c r="C3" s="6">
         <v>1.0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>265.82</v>
       </c>
       <c r="E3" s="6">
@@ -670,7 +685,7 @@
       <c r="O3" s="6">
         <v>1.0</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="4">
         <v>303.03</v>
       </c>
       <c r="Q3" s="6">
@@ -682,15 +697,15 @@
       <c r="S3" s="6">
         <v>1.0</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="5">
         <v>595510.630882847</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3" s="5">
         <v>6740736.35252594</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="7">
@@ -722,8 +737,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
+      <c r="A5" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B5" s="7">
         <v>374.3</v>
@@ -731,13 +746,13 @@
       <c r="C5" s="6">
         <v>1.0</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>344.44</v>
       </c>
       <c r="E5" s="6">
         <v>0.0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>324.02</v>
       </c>
       <c r="G5" s="6">
@@ -779,18 +794,18 @@
       <c r="S5" s="6">
         <v>1.0</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="5">
         <v>596454.888567045</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="5">
         <v>6739984.58756568</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>407.89</v>
       </c>
       <c r="C6" s="6">
@@ -818,7 +833,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="7">
@@ -855,19 +870,19 @@
       <c r="B8" s="10">
         <v>335.94</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>1.0</v>
       </c>
       <c r="D8" s="10">
         <v>328.13</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>1.0</v>
       </c>
       <c r="F8" s="11">
         <v>169.23</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="1">
         <v>0.0</v>
       </c>
       <c r="H8" s="12"/>
@@ -888,12 +903,12 @@
       <c r="U8" s="10">
         <v>6741167.0</v>
       </c>
-      <c r="V8" s="3">
+      <c r="V8" s="1">
         <v>2332.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="7">
@@ -908,7 +923,7 @@
       <c r="E9" s="6">
         <v>1.0</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>241.38</v>
       </c>
       <c r="G9" s="6">
@@ -922,10 +937,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="5">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4">
         <v>160.38</v>
       </c>
       <c r="C10" s="6">
@@ -967,7 +982,7 @@
       <c r="O10" s="6">
         <v>1.0</v>
       </c>
-      <c r="P10" s="5">
+      <c r="P10" s="4">
         <v>290.32</v>
       </c>
       <c r="Q10" s="6">
@@ -979,15 +994,15 @@
       <c r="S10" s="6">
         <v>1.0</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T10" s="5">
         <v>600044.719257886</v>
       </c>
-      <c r="U10" s="2">
+      <c r="U10" s="5">
         <v>6754368.04943599</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="7">
@@ -1016,7 +1031,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="7">
@@ -1045,798 +1060,884 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="7">
         <v>299.21</v>
       </c>
-      <c r="C13" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="10">
+      <c r="C13" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="7">
         <v>295.45</v>
       </c>
-      <c r="E13" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F13" s="10">
+      <c r="E13" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="7">
         <v>306.45</v>
       </c>
-      <c r="G13" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="10">
+      <c r="G13" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T13" s="7">
         <v>600852.0</v>
       </c>
-      <c r="U13" s="10">
+      <c r="U13" s="7">
         <v>6753799.0</v>
       </c>
-      <c r="V13" s="12"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="13">
+        <v>246.3337709447</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D14" s="13">
+        <v>251.3609907599</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>232.2338581297</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T14" s="13">
+        <v>598954.0</v>
+      </c>
+      <c r="U14" s="13">
+        <v>6755390.0</v>
+      </c>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="14">
+        <v>263.46</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="14">
+        <v>261.26</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F15" s="15">
+        <v>231.66</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="H15" s="14">
+        <v>261.26</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J15" s="14">
+        <v>234.19</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="L15" s="14">
+        <v>233.68</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="N15" s="14">
+        <v>257.12</v>
+      </c>
+      <c r="O15" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="P15" s="14">
+        <v>245.79</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="16">
+        <v>598830.956870471</v>
+      </c>
+      <c r="U15" s="16">
+        <v>6755272.76759809</v>
+      </c>
+      <c r="V15" s="12"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="7">
         <v>346.67</v>
       </c>
-      <c r="C14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="C16" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D16" s="7">
         <v>344.83</v>
       </c>
-      <c r="E14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F14" s="7">
+      <c r="E16" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F16" s="7">
         <v>351.35</v>
       </c>
-      <c r="G14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="H14" s="7">
+      <c r="G16" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="H16" s="7">
         <v>342.28</v>
       </c>
-      <c r="I14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="J14" s="7">
+      <c r="I16" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="J16" s="7">
         <v>350.36</v>
       </c>
-      <c r="K14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="L14" s="7">
+      <c r="K16" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="L16" s="7">
         <v>350.36</v>
       </c>
-      <c r="M14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="N14" s="7">
+      <c r="M16" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="N16" s="7">
         <v>360.54</v>
       </c>
-      <c r="O14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="P14" s="7">
+      <c r="O16" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="P16" s="7">
         <v>344.83</v>
       </c>
-      <c r="Q14" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="T14" s="2">
+      <c r="Q16" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T16" s="5">
         <v>595126.583444399</v>
       </c>
-      <c r="U14" s="2">
+      <c r="U16" s="5">
         <v>6742232.89922962</v>
       </c>
-      <c r="V14" s="7">
+      <c r="V16" s="7">
         <v>2517.0</v>
       </c>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="5">
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="4">
         <v>294.57</v>
       </c>
-      <c r="C15" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D15" s="5">
+      <c r="C17" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D17" s="4">
         <v>286.82</v>
       </c>
-      <c r="E15" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="F15" s="5">
+      <c r="E17" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="4">
         <v>322.83</v>
       </c>
-      <c r="G15" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="M15" s="6"/>
-      <c r="T15" s="2">
+      <c r="G17" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="6"/>
+      <c r="T17" s="5">
         <v>606370.157387766</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U17" s="5">
         <v>6761967.14383023</v>
       </c>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="7">
-        <v>344.83</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D16" s="7">
-        <v>366.67</v>
-      </c>
-      <c r="E16" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F16" s="7">
-        <v>343.64</v>
-      </c>
-      <c r="G16" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="T16" s="7">
-        <v>606318.0</v>
-      </c>
-      <c r="U16" s="7">
-        <v>6761532.0</v>
-      </c>
-      <c r="V16" s="7">
-        <v>2524.0</v>
-      </c>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="2"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="5">
-        <v>324.32</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D17" s="7">
-        <v>330.43</v>
-      </c>
-      <c r="E17" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F17" s="7">
-        <v>355.56</v>
-      </c>
-      <c r="G17" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="H17" s="8">
-        <v>326.09</v>
-      </c>
-      <c r="I17" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="T17" s="7">
-        <v>606299.0</v>
-      </c>
-      <c r="U17" s="7">
-        <v>6741270.0</v>
-      </c>
-      <c r="V17" s="7">
-        <v>2535.0</v>
-      </c>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="2"/>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="5">
-        <v>307.09</v>
+        <v>45</v>
+      </c>
+      <c r="B18" s="7">
+        <v>344.83</v>
       </c>
       <c r="C18" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>339.92</v>
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="7">
+        <v>366.67</v>
       </c>
       <c r="E18" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="F18" s="5">
-        <v>338.35</v>
+        <v>1.0</v>
+      </c>
+      <c r="F18" s="7">
+        <v>343.64</v>
       </c>
       <c r="G18" s="6">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="T18" s="7">
-        <v>606275.0</v>
+        <v>606318.0</v>
       </c>
       <c r="U18" s="7">
-        <v>6760989.0</v>
+        <v>6761532.0</v>
       </c>
       <c r="V18" s="7">
-        <v>2546.0</v>
-      </c>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="2"/>
+        <v>2524.0</v>
+      </c>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="7">
-        <v>386.55</v>
+        <v>46</v>
+      </c>
+      <c r="B19" s="4">
+        <v>324.32</v>
       </c>
       <c r="C19" s="6">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D19" s="7">
-        <v>323.53</v>
+        <v>330.43</v>
       </c>
       <c r="E19" s="6">
         <v>1.0</v>
       </c>
       <c r="F19" s="7">
-        <v>294.12</v>
+        <v>355.56</v>
       </c>
       <c r="G19" s="6">
         <v>1.0</v>
       </c>
+      <c r="H19" s="8">
+        <v>326.09</v>
+      </c>
+      <c r="I19" s="6">
+        <v>1.0</v>
+      </c>
       <c r="T19" s="7">
-        <v>606253.0</v>
+        <v>606299.0</v>
       </c>
       <c r="U19" s="7">
-        <v>6760715.0</v>
+        <v>6741270.0</v>
       </c>
       <c r="V19" s="7">
-        <v>2573.0</v>
-      </c>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="2"/>
+        <v>2535.0</v>
+      </c>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="7">
-        <v>340.43</v>
+        <v>47</v>
+      </c>
+      <c r="B20" s="4">
+        <v>307.09</v>
       </c>
       <c r="C20" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D20" s="5">
-        <v>363.64</v>
+        <v>0.0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>339.92</v>
       </c>
       <c r="E20" s="6">
         <v>0.0</v>
       </c>
-      <c r="F20" s="5">
-        <v>217.39</v>
+      <c r="F20" s="4">
+        <v>338.35</v>
       </c>
       <c r="G20" s="6">
         <v>0.0</v>
       </c>
       <c r="T20" s="7">
-        <v>606397.0</v>
+        <v>606275.0</v>
       </c>
       <c r="U20" s="7">
-        <v>6761622.0</v>
+        <v>6760989.0</v>
       </c>
       <c r="V20" s="7">
-        <v>2532.0</v>
-      </c>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="2"/>
+        <v>2546.0</v>
+      </c>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="7">
-        <v>313.25</v>
+        <v>386.55</v>
       </c>
       <c r="C21" s="6">
         <v>1.0</v>
       </c>
       <c r="D21" s="7">
-        <v>333.33</v>
+        <v>323.53</v>
       </c>
       <c r="E21" s="6">
         <v>1.0</v>
       </c>
       <c r="F21" s="7">
-        <v>362.75</v>
+        <v>294.12</v>
       </c>
       <c r="G21" s="6">
         <v>1.0</v>
       </c>
       <c r="T21" s="7">
-        <v>606142.0</v>
+        <v>606253.0</v>
       </c>
       <c r="U21" s="7">
-        <v>6761205.0</v>
+        <v>6760715.0</v>
       </c>
       <c r="V21" s="7">
-        <v>2526.0</v>
-      </c>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="2"/>
-      <c r="AA21" s="2"/>
-      <c r="AB21" s="2"/>
+        <v>2573.0</v>
+      </c>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="7">
-        <v>328.77</v>
+        <v>340.43</v>
       </c>
       <c r="C22" s="6">
         <v>1.0</v>
       </c>
-      <c r="D22" s="7">
-        <v>263.16</v>
+      <c r="D22" s="4">
+        <v>363.64</v>
       </c>
       <c r="E22" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F22" s="7">
-        <v>320.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>217.39</v>
       </c>
       <c r="G22" s="6">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="T22" s="7">
-        <v>606083.0</v>
+        <v>606397.0</v>
       </c>
       <c r="U22" s="7">
-        <v>6762163.0</v>
+        <v>6761622.0</v>
       </c>
       <c r="V22" s="7">
-        <v>2483.0</v>
-      </c>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="2"/>
+        <v>2532.0</v>
+      </c>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="7">
-        <v>303.28</v>
+        <v>313.25</v>
       </c>
       <c r="C23" s="6">
         <v>1.0</v>
       </c>
-      <c r="D23" s="5">
-        <v>204.38</v>
+      <c r="D23" s="7">
+        <v>333.33</v>
       </c>
       <c r="E23" s="6">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F23" s="7">
-        <v>335.71</v>
+        <v>362.75</v>
       </c>
       <c r="G23" s="6">
         <v>1.0</v>
       </c>
       <c r="T23" s="7">
-        <v>605969.0</v>
+        <v>606142.0</v>
       </c>
       <c r="U23" s="7">
-        <v>6762550.0</v>
+        <v>6761205.0</v>
       </c>
       <c r="V23" s="7">
-        <v>2419.0</v>
-      </c>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="2"/>
-      <c r="AA23" s="2"/>
-      <c r="AB23" s="2"/>
+        <v>2526.0</v>
+      </c>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="7">
+        <v>328.77</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="7">
+        <v>263.16</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F24" s="7">
+        <v>320.0</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T24" s="7">
+        <v>606083.0</v>
+      </c>
+      <c r="U24" s="7">
+        <v>6762163.0</v>
+      </c>
+      <c r="V24" s="7">
+        <v>2483.0</v>
+      </c>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="5"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B25" s="7">
+        <v>303.28</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>204.38</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F25" s="7">
+        <v>335.71</v>
+      </c>
+      <c r="G25" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T25" s="7">
+        <v>605969.0</v>
+      </c>
+      <c r="U25" s="7">
+        <v>6762550.0</v>
+      </c>
+      <c r="V25" s="7">
+        <v>2419.0</v>
+      </c>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="7">
         <v>303.92</v>
       </c>
-      <c r="C24" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D24" s="7">
+      <c r="C26" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D26" s="7">
         <v>331.75</v>
       </c>
-      <c r="E24" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F24" s="7">
+      <c r="E26" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F26" s="7">
         <v>307.69</v>
       </c>
-      <c r="G24" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="T24" s="7">
+      <c r="G26" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T26" s="7">
         <v>605121.0</v>
       </c>
-      <c r="U24" s="7">
+      <c r="U26" s="7">
         <v>6762899.0</v>
       </c>
-      <c r="V24" s="7">
+      <c r="V26" s="7">
         <v>2321.0</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="8">
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="8">
         <v>247.19</v>
       </c>
-      <c r="C25" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D25" s="7">
+      <c r="C27" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D27" s="7">
         <v>277.11</v>
       </c>
-      <c r="E25" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F25" s="7">
+      <c r="E27" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F27" s="7">
         <v>271.6</v>
       </c>
-      <c r="G25" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="T25" s="7">
+      <c r="G27" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T27" s="7">
         <v>604708.0</v>
       </c>
-      <c r="U25" s="7">
+      <c r="U27" s="7">
         <v>6762812.0</v>
       </c>
-      <c r="V25" s="13">
+      <c r="V27" s="17">
         <v>2296.0</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="7">
+    <row r="28">
+      <c r="A28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="7">
         <v>310.34</v>
       </c>
-      <c r="C26" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D26" s="7">
+      <c r="C28" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D28" s="7">
         <v>327.49</v>
       </c>
-      <c r="E26" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F26" s="7">
+      <c r="E28" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F28" s="7">
         <v>328.77</v>
       </c>
-      <c r="G26" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="H26" s="7">
+      <c r="G28" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="H28" s="7">
         <v>331.13</v>
       </c>
-      <c r="I26" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="J26" s="8">
+      <c r="I28" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="J28" s="8">
         <v>262.5</v>
       </c>
-      <c r="K26" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="L26" s="8">
+      <c r="K28" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="L28" s="8">
         <v>259.26</v>
       </c>
-      <c r="M26" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="N26" s="7">
+      <c r="M28" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="N28" s="7">
         <v>301.2</v>
       </c>
-      <c r="O26" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="P26" s="7">
+      <c r="O28" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="P28" s="7">
         <v>301.2</v>
       </c>
-      <c r="Q26" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="T26" s="2">
+      <c r="Q28" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T28" s="5">
         <v>604509.073083514</v>
       </c>
-      <c r="U26" s="2">
+      <c r="U28" s="5">
         <v>6763342.34093057</v>
       </c>
-      <c r="V26" s="7">
+      <c r="V28" s="7">
         <v>2257.0</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="5">
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="4">
         <v>370.08</v>
       </c>
-      <c r="C27" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D27" s="7">
+      <c r="C29" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D29" s="7">
         <v>407.69</v>
       </c>
-      <c r="E27" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F27" s="5">
+      <c r="E29" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F29" s="4">
         <v>488.37</v>
       </c>
-      <c r="G27" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="T27" s="7">
+      <c r="G29" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="T29" s="7">
         <v>603904.0</v>
       </c>
-      <c r="U27" s="7">
+      <c r="U29" s="7">
         <v>6764001.0</v>
       </c>
-      <c r="V27" s="13">
+      <c r="V29" s="17">
         <v>2206.0</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="7">
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="7">
         <v>250.0</v>
       </c>
-      <c r="C28" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D28" s="7">
+      <c r="C30" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D30" s="7">
         <v>225.0</v>
       </c>
-      <c r="E28" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F28" s="7">
+      <c r="E30" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F30" s="7">
         <v>243.9</v>
       </c>
-      <c r="G28" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="T28" s="7">
+      <c r="G30" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T30" s="7">
         <v>603925.0</v>
       </c>
-      <c r="U28" s="7">
+      <c r="U30" s="7">
         <v>6764029.0</v>
       </c>
-      <c r="V28" s="7">
+      <c r="V30" s="7">
         <v>2206.0</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="7">
+    <row r="31">
+      <c r="A31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="7">
         <v>275.0</v>
       </c>
-      <c r="C29" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D29" s="7">
+      <c r="C31" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D31" s="7">
         <v>268.29</v>
       </c>
-      <c r="E29" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F29" s="6">
+      <c r="E31" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F31" s="6">
         <v>260.87</v>
       </c>
-      <c r="G29" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="T29" s="7">
+      <c r="G31" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T31" s="7">
         <v>603569.0</v>
       </c>
-      <c r="U29" s="7">
+      <c r="U31" s="7">
         <v>6764536.0</v>
       </c>
-      <c r="V29" s="13">
+      <c r="V31" s="17">
         <v>2156.0</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="7">
+    <row r="32">
+      <c r="A32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="7">
         <v>274.51</v>
       </c>
-      <c r="C30" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D30" s="5">
+      <c r="C32" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D32" s="4">
         <v>207.55</v>
       </c>
-      <c r="E30" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="F30" s="7">
+      <c r="E32" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F32" s="7">
         <v>306.12</v>
       </c>
-      <c r="G30" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="T30" s="7">
+      <c r="G32" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T32" s="7">
         <v>603927.0</v>
       </c>
-      <c r="U30" s="7">
+      <c r="U32" s="7">
         <v>6764001.0</v>
       </c>
-      <c r="V30" s="13">
+      <c r="V32" s="17">
         <v>2214.0</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="7">
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="7">
         <v>277.78</v>
       </c>
-      <c r="C31" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D31" s="7">
+      <c r="C33" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D33" s="7">
         <v>273.68</v>
       </c>
-      <c r="E31" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F31" s="5">
+      <c r="E33" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F33" s="4">
         <v>236.02</v>
       </c>
-      <c r="G31" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="H31" s="7">
+      <c r="G33" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="H33" s="7">
         <v>243.09</v>
       </c>
-      <c r="I31" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="T31" s="7">
+      <c r="I33" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T33" s="7">
         <v>604583.0</v>
       </c>
-      <c r="U31" s="7">
+      <c r="U33" s="7">
         <v>6763779.0</v>
       </c>
-      <c r="V31" s="13">
+      <c r="V33" s="17">
         <v>2246.0</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="5">
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="4">
         <v>276.32</v>
       </c>
-      <c r="C32" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D32" s="7">
+      <c r="C34" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="D34" s="7">
         <v>318.47</v>
       </c>
-      <c r="E32" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F32" s="5">
+      <c r="E34" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="F34" s="4">
         <v>251.66</v>
       </c>
-      <c r="G32" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="H32" s="7">
+      <c r="G34" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="H34" s="7">
         <v>324.68</v>
       </c>
-      <c r="I32" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="T32" s="7">
+      <c r="I34" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="T34" s="7">
         <v>603843.0</v>
       </c>
-      <c r="U32" s="7">
+      <c r="U34" s="7">
         <v>6763492.0</v>
       </c>
-      <c r="V32" s="13">
+      <c r="V34" s="17">
         <v>2216.0</v>
       </c>
     </row>
-    <row r="34">
-      <c r="T34" s="14"/>
-      <c r="U34" s="14"/>
-      <c r="V34" s="14"/>
-    </row>
-    <row r="35">
-      <c r="T35" s="14"/>
-      <c r="U35" s="14"/>
-      <c r="V35" s="14"/>
+    <row r="36">
+      <c r="T36" s="18"/>
+      <c r="U36" s="18"/>
+      <c r="V36" s="18"/>
     </row>
     <row r="37">
-      <c r="T37" s="14"/>
-      <c r="U37" s="14"/>
-      <c r="V37" s="14"/>
-    </row>
-    <row r="38">
-      <c r="T38" s="14"/>
-      <c r="U38" s="14"/>
-      <c r="V38" s="14"/>
+      <c r="T37" s="18"/>
+      <c r="U37" s="18"/>
+      <c r="V37" s="18"/>
+    </row>
+    <row r="39">
+      <c r="T39" s="18"/>
+      <c r="U39" s="18"/>
+      <c r="V39" s="18"/>
     </row>
     <row r="40">
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-      <c r="V40" s="14"/>
-    </row>
-    <row r="41">
-      <c r="T41" s="14"/>
-      <c r="U41" s="14"/>
-      <c r="V41" s="14"/>
+      <c r="T40" s="18"/>
+      <c r="U40" s="18"/>
+      <c r="V40" s="18"/>
+    </row>
+    <row r="42">
+      <c r="T42" s="18"/>
+      <c r="U42" s="18"/>
+      <c r="V42" s="18"/>
+    </row>
+    <row r="43">
+      <c r="T43" s="18"/>
+      <c r="U43" s="18"/>
+      <c r="V43" s="18"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Adding transect ANOVA and density plots
</commit_message>
<xml_diff>
--- a/summary_densitydata.xlsx
+++ b/summary_densitydata.xlsx
@@ -12,11 +12,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>elev</t>
+  </si>
+  <si>
     <t>SWE1</t>
   </si>
   <si>
@@ -71,21 +83,9 @@
     <t>Q9</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>elev</t>
-  </si>
-  <si>
     <t>G04_Z3A_SWE</t>
   </si>
   <si>
-    <t>density</t>
-  </si>
-  <si>
     <t>G02_LSP</t>
   </si>
   <si>
@@ -140,13 +140,10 @@
     <t>G02_Z7C_SWE</t>
   </si>
   <si>
-    <t>G03_Z3B_SWE</t>
-  </si>
-  <si>
-    <t>GL13_ASP</t>
-  </si>
-  <si>
-    <t>GL13_AFC05</t>
+    <t>G02_Z3B_SWE</t>
+  </si>
+  <si>
+    <t>G13_AFC05</t>
   </si>
   <si>
     <t>G13_651</t>
@@ -177,9 +174,6 @@
   </si>
   <si>
     <t>G13_Z7C_SWE</t>
-  </si>
-  <si>
-    <t>G13_USP_SWE</t>
   </si>
   <si>
     <t>G13_Z4C_SWE</t>
@@ -263,23 +257,23 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
@@ -339,21 +333,24 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="5">
@@ -365,9 +362,12 @@
       <c r="D2" s="5">
         <v>6755272.76759921</v>
       </c>
+      <c r="E2" s="3">
+        <v>2175.0</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="5">
@@ -379,9 +379,12 @@
       <c r="D3" s="5">
         <v>6754686.13</v>
       </c>
+      <c r="E3" s="3">
+        <v>2261.0</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="5">
@@ -393,9 +396,12 @@
       <c r="D4" s="5">
         <v>6754368.04943599</v>
       </c>
+      <c r="E4" s="3">
+        <v>2349.0</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="5">
@@ -407,9 +413,12 @@
       <c r="D5" s="5">
         <v>6753115.5549246</v>
       </c>
+      <c r="E5" s="3">
+        <v>2550.0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="5">
@@ -421,9 +430,12 @@
       <c r="D6" s="5">
         <v>6739984.58756568</v>
       </c>
+      <c r="E6" s="3">
+        <v>2154.0</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="5">
@@ -435,9 +447,12 @@
       <c r="D7" s="5">
         <v>6740736.35252594</v>
       </c>
+      <c r="E7" s="3">
+        <v>2298.0</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="5">
@@ -449,9 +464,12 @@
       <c r="D8" s="5">
         <v>6742232.89922962</v>
       </c>
+      <c r="E8" s="3">
+        <v>2482.0</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="5">
@@ -463,9 +481,12 @@
       <c r="D9" s="5">
         <v>6764638.61521979</v>
       </c>
+      <c r="E9" s="3">
+        <v>2139.0</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="5">
@@ -477,9 +498,12 @@
       <c r="D10" s="5">
         <v>6763342.34093057</v>
       </c>
+      <c r="E10" s="3">
+        <v>2257.0</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="5">
@@ -490,6 +514,9 @@
       </c>
       <c r="D11" s="5">
         <v>6761736.67808849</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2516.0</v>
       </c>
     </row>
   </sheetData>
@@ -526,105 +553,105 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6">
         <v>321.05</v>
       </c>
-      <c r="C2" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="6">
         <v>321.24</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="3">
         <v>0.0</v>
       </c>
       <c r="F2" s="7">
         <v>361.26</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="3">
         <v>1.0</v>
       </c>
       <c r="H2" s="7">
         <v>378.95</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="3">
         <v>1.0</v>
       </c>
       <c r="J2" s="7">
         <v>370.56</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="3">
         <v>1.0</v>
       </c>
       <c r="R2" s="7"/>
@@ -640,61 +667,61 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="8">
         <v>322.98</v>
       </c>
-      <c r="C3" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="6">
         <v>265.82</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="3">
         <v>0.0</v>
       </c>
       <c r="F3" s="7">
         <v>355.03</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="3">
         <v>1.0</v>
       </c>
       <c r="H3" s="7">
         <v>363.64</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="3">
         <v>1.0</v>
       </c>
       <c r="J3" s="7">
         <v>364.16</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="3">
         <v>1.0</v>
       </c>
       <c r="L3" s="7">
         <v>327.59</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="3">
         <v>1.0</v>
       </c>
       <c r="N3" s="7">
         <v>337.35</v>
       </c>
-      <c r="O3" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="P3" s="4">
+      <c r="O3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="P3" s="6">
         <v>303.03</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="Q3" s="3">
         <v>0.0</v>
       </c>
       <c r="R3" s="7">
         <v>363.1</v>
       </c>
-      <c r="S3" s="6">
+      <c r="S3" s="3">
         <v>1.0</v>
       </c>
       <c r="T3" s="5">
@@ -703,30 +730,33 @@
       <c r="U3" s="5">
         <v>6740736.35252594</v>
       </c>
+      <c r="V3" s="3">
+        <v>2298.0</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="7">
         <v>352.94</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>1.0</v>
       </c>
       <c r="D4" s="7">
         <v>374.33</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
         <v>1.0</v>
       </c>
       <c r="F4" s="7">
         <v>377.14</v>
       </c>
-      <c r="G4" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="I4" s="6"/>
+      <c r="G4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I4" s="3"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="T4" s="7">
@@ -735,63 +765,66 @@
       <c r="U4" s="7">
         <v>6739965.0</v>
       </c>
+      <c r="V4" s="3">
+        <v>2162.0</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="7">
         <v>374.3</v>
       </c>
-      <c r="C5" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="6">
         <v>344.44</v>
       </c>
-      <c r="E5" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="E5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="6">
         <v>324.02</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="3">
         <v>0.0</v>
       </c>
       <c r="H5" s="7">
         <v>372.34</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="3">
         <v>1.0</v>
       </c>
       <c r="J5" s="7">
         <v>376.34</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="3">
         <v>1.0</v>
       </c>
       <c r="L5" s="7">
         <v>372.97</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="3">
         <v>1.0</v>
       </c>
       <c r="N5" s="7">
         <v>362.16</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="3">
         <v>1.0</v>
       </c>
       <c r="P5" s="7">
         <v>375.66</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="3">
         <v>1.0</v>
       </c>
       <c r="R5" s="7">
         <v>372.97</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S5" s="3">
         <v>1.0</v>
       </c>
       <c r="T5" s="5">
@@ -800,27 +833,30 @@
       <c r="U5" s="5">
         <v>6739984.58756568</v>
       </c>
+      <c r="V5" s="3">
+        <v>2154.0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>407.89</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>0.0</v>
       </c>
       <c r="D6" s="7">
         <v>362.57</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="3">
         <v>1.0</v>
       </c>
       <c r="F6" s="7">
         <v>356.32</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="3">
         <v>1.0</v>
       </c>
       <c r="R6" s="7"/>
@@ -831,27 +867,30 @@
       <c r="U6" s="7">
         <v>6741154.0</v>
       </c>
+      <c r="V6" s="3">
+        <v>2360.0</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="7">
         <v>329.9</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>1.0</v>
       </c>
       <c r="D7" s="7">
         <v>331.63</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="3">
         <v>1.0</v>
       </c>
       <c r="F7" s="7">
         <v>321.24</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="3">
         <v>1.0</v>
       </c>
       <c r="R7" s="7"/>
@@ -862,6 +901,9 @@
       <c r="U7" s="7">
         <v>6740736.0</v>
       </c>
+      <c r="V7" s="3">
+        <v>2328.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
@@ -870,19 +912,19 @@
       <c r="B8" s="10">
         <v>335.94</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>1.0</v>
       </c>
       <c r="D8" s="10">
         <v>328.13</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>1.0</v>
       </c>
       <c r="F8" s="11">
         <v>169.23</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>0.0</v>
       </c>
       <c r="H8" s="12"/>
@@ -903,30 +945,30 @@
       <c r="U8" s="10">
         <v>6741167.0</v>
       </c>
-      <c r="V8" s="1">
+      <c r="V8" s="2">
         <v>2332.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="7">
         <v>283.19</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="3">
         <v>1.0</v>
       </c>
       <c r="D9" s="7">
         <v>263.64</v>
       </c>
-      <c r="E9" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F9" s="4">
+      <c r="E9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="6">
         <v>241.38</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="3">
         <v>0.0</v>
       </c>
       <c r="T9" s="7">
@@ -935,63 +977,66 @@
       <c r="U9" s="7">
         <v>6754533.0</v>
       </c>
+      <c r="V9" s="3">
+        <v>2332.0</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="6">
         <v>160.38</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="3">
         <v>0.0</v>
       </c>
       <c r="D10" s="7">
         <v>269.23</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="3">
         <v>1.0</v>
       </c>
       <c r="F10" s="7">
         <v>271.84</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="3">
         <v>1.0</v>
       </c>
       <c r="H10" s="7">
         <v>268.52</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="3">
         <v>1.0</v>
       </c>
       <c r="J10" s="7">
         <v>266.67</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="3">
         <v>1.0</v>
       </c>
       <c r="L10" s="7">
         <v>300.0</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="3">
         <v>1.0</v>
       </c>
       <c r="N10" s="7">
         <v>299.15</v>
       </c>
-      <c r="O10" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="P10" s="4">
+      <c r="O10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="P10" s="6">
         <v>290.32</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="3">
         <v>0.0</v>
       </c>
       <c r="R10" s="7">
         <v>307.69</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="3">
         <v>1.0</v>
       </c>
       <c r="T10" s="5">
@@ -1000,27 +1045,30 @@
       <c r="U10" s="5">
         <v>6754368.04943599</v>
       </c>
+      <c r="V10" s="3">
+        <v>2349.0</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="7">
         <v>326.02</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>1.0</v>
       </c>
       <c r="D11" s="7">
         <v>369.39</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="3">
         <v>1.0</v>
       </c>
       <c r="F11" s="7">
         <v>329.27</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="3">
         <v>1.0</v>
       </c>
       <c r="T11" s="7">
@@ -1029,27 +1077,30 @@
       <c r="U11" s="7">
         <v>6754216.0</v>
       </c>
+      <c r="V11" s="3">
+        <v>2403.0</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="7">
         <v>302.63</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>1.0</v>
       </c>
       <c r="D12" s="8">
         <v>291.39</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="3">
         <v>1.0</v>
       </c>
       <c r="F12" s="7">
         <v>309.21</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="3">
         <v>1.0</v>
       </c>
       <c r="T12" s="7">
@@ -1058,27 +1109,30 @@
       <c r="U12" s="7">
         <v>6754169.0</v>
       </c>
+      <c r="V12" s="3">
+        <v>2458.0</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="7">
         <v>299.21</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="3">
         <v>1.0</v>
       </c>
       <c r="D13" s="7">
         <v>295.45</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="3">
         <v>1.0</v>
       </c>
       <c r="F13" s="7">
         <v>306.45</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="3">
         <v>1.0</v>
       </c>
       <c r="T13" s="7">
@@ -1087,31 +1141,34 @@
       <c r="U13" s="7">
         <v>6753799.0</v>
       </c>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
+      <c r="V13" s="3">
+        <v>2442.0</v>
+      </c>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="13">
         <v>246.3337709447</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="3">
         <v>1.0</v>
       </c>
       <c r="D14" s="13">
         <v>251.3609907599</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="3">
         <v>1.0</v>
       </c>
       <c r="F14" s="13">
         <v>232.2338581297</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="3">
         <v>1.0</v>
       </c>
       <c r="T14" s="13">
@@ -1120,10 +1177,13 @@
       <c r="U14" s="13">
         <v>6755390.0</v>
       </c>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="3"/>
+      <c r="V14" s="3">
+        <v>2172.0</v>
+      </c>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
@@ -1132,49 +1192,49 @@
       <c r="B15" s="14">
         <v>263.46</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>1.0</v>
       </c>
       <c r="D15" s="14">
         <v>261.26</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2">
         <v>1.0</v>
       </c>
       <c r="F15" s="15">
         <v>231.66</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <v>0.0</v>
       </c>
       <c r="H15" s="14">
         <v>261.26</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="2">
         <v>1.0</v>
       </c>
       <c r="J15" s="14">
         <v>234.19</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="2">
         <v>1.0</v>
       </c>
       <c r="L15" s="14">
         <v>233.68</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="2">
         <v>1.0</v>
       </c>
       <c r="N15" s="14">
         <v>257.12</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="2">
         <v>1.0</v>
       </c>
       <c r="P15" s="14">
         <v>245.79</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="Q15" s="2">
         <v>1.0</v>
       </c>
       <c r="R15" s="12"/>
@@ -1185,62 +1245,64 @@
       <c r="U15" s="16">
         <v>6755272.76759809</v>
       </c>
-      <c r="V15" s="12"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
-      <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
+      <c r="V15" s="2">
+        <v>2175.0</v>
+      </c>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>43</v>
+      <c r="A16" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B16" s="7">
         <v>346.67</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="3">
         <v>1.0</v>
       </c>
       <c r="D16" s="7">
         <v>344.83</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="3">
         <v>1.0</v>
       </c>
       <c r="F16" s="7">
         <v>351.35</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="3">
         <v>1.0</v>
       </c>
       <c r="H16" s="7">
         <v>342.28</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="3">
         <v>1.0</v>
       </c>
       <c r="J16" s="7">
         <v>350.36</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="3">
         <v>1.0</v>
       </c>
       <c r="L16" s="7">
         <v>350.36</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="3">
         <v>1.0</v>
       </c>
       <c r="N16" s="7">
         <v>360.54</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="3">
         <v>1.0</v>
       </c>
       <c r="P16" s="7">
         <v>344.83</v>
       </c>
-      <c r="Q16" s="6">
+      <c r="Q16" s="3">
         <v>1.0</v>
       </c>
       <c r="T16" s="5">
@@ -1252,65 +1314,65 @@
       <c r="V16" s="7">
         <v>2517.0</v>
       </c>
-      <c r="Y16" s="3"/>
+      <c r="Y16" s="1"/>
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="4">
+      <c r="A17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="6">
         <v>294.57</v>
       </c>
-      <c r="C17" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="C17" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D17" s="6">
         <v>286.82</v>
       </c>
-      <c r="E17" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="F17" s="4">
+      <c r="E17" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="6">
         <v>322.83</v>
       </c>
-      <c r="G17" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="M17" s="6"/>
+      <c r="G17" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="3"/>
       <c r="T17" s="5">
         <v>606370.157387766</v>
       </c>
       <c r="U17" s="5">
         <v>6761967.14383023</v>
       </c>
-      <c r="Y17" s="3"/>
+      <c r="Y17" s="1"/>
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>45</v>
+      <c r="A18" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B18" s="7">
         <v>344.83</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="3">
         <v>1.0</v>
       </c>
       <c r="D18" s="7">
         <v>366.67</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="3">
         <v>1.0</v>
       </c>
       <c r="F18" s="7">
         <v>343.64</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="3">
         <v>1.0</v>
       </c>
       <c r="T18" s="7">
@@ -1322,37 +1384,37 @@
       <c r="V18" s="7">
         <v>2524.0</v>
       </c>
-      <c r="Y18" s="3"/>
+      <c r="Y18" s="1"/>
       <c r="Z18" s="5"/>
       <c r="AA18" s="5"/>
       <c r="AB18" s="5"/>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="4">
+      <c r="A19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="6">
         <v>324.32</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="3">
         <v>0.0</v>
       </c>
       <c r="D19" s="7">
         <v>330.43</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="3">
         <v>1.0</v>
       </c>
       <c r="F19" s="7">
         <v>355.56</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="3">
         <v>1.0</v>
       </c>
       <c r="H19" s="8">
         <v>326.09</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="3">
         <v>1.0</v>
       </c>
       <c r="T19" s="7">
@@ -1364,31 +1426,31 @@
       <c r="V19" s="7">
         <v>2535.0</v>
       </c>
-      <c r="Y19" s="3"/>
+      <c r="Y19" s="1"/>
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="4">
+      <c r="A20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="6">
         <v>307.09</v>
       </c>
-      <c r="C20" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="C20" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D20" s="6">
         <v>339.92</v>
       </c>
-      <c r="E20" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="F20" s="4">
+      <c r="E20" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F20" s="6">
         <v>338.35</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="3">
         <v>0.0</v>
       </c>
       <c r="T20" s="7">
@@ -1400,29 +1462,29 @@
       <c r="V20" s="7">
         <v>2546.0</v>
       </c>
-      <c r="Y20" s="3"/>
+      <c r="Y20" s="1"/>
       <c r="Z20" s="5"/>
     </row>
     <row r="21">
-      <c r="A21" s="6" t="s">
-        <v>48</v>
+      <c r="A21" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B21" s="7">
         <v>386.55</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="3">
         <v>1.0</v>
       </c>
       <c r="D21" s="7">
         <v>323.53</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="3">
         <v>1.0</v>
       </c>
       <c r="F21" s="7">
         <v>294.12</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="3">
         <v>1.0</v>
       </c>
       <c r="T21" s="7">
@@ -1434,29 +1496,29 @@
       <c r="V21" s="7">
         <v>2573.0</v>
       </c>
-      <c r="Y21" s="3"/>
+      <c r="Y21" s="1"/>
       <c r="Z21" s="5"/>
     </row>
     <row r="22">
-      <c r="A22" s="6" t="s">
-        <v>49</v>
+      <c r="A22" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="B22" s="7">
         <v>340.43</v>
       </c>
-      <c r="C22" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D22" s="4">
+      <c r="C22" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D22" s="6">
         <v>363.64</v>
       </c>
-      <c r="E22" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="F22" s="4">
+      <c r="E22" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F22" s="6">
         <v>217.39</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="3">
         <v>0.0</v>
       </c>
       <c r="T22" s="7">
@@ -1468,31 +1530,31 @@
       <c r="V22" s="7">
         <v>2532.0</v>
       </c>
-      <c r="Y22" s="3"/>
+      <c r="Y22" s="1"/>
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="s">
-        <v>50</v>
+      <c r="A23" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B23" s="7">
         <v>313.25</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="3">
         <v>1.0</v>
       </c>
       <c r="D23" s="7">
         <v>333.33</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="3">
         <v>1.0</v>
       </c>
       <c r="F23" s="7">
         <v>362.75</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="3">
         <v>1.0</v>
       </c>
       <c r="T23" s="7">
@@ -1504,31 +1566,31 @@
       <c r="V23" s="7">
         <v>2526.0</v>
       </c>
-      <c r="Y23" s="3"/>
+      <c r="Y23" s="1"/>
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
       <c r="AB23" s="5"/>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="s">
-        <v>51</v>
+      <c r="A24" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B24" s="7">
         <v>328.77</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="3">
         <v>1.0</v>
       </c>
       <c r="D24" s="7">
         <v>263.16</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="3">
         <v>1.0</v>
       </c>
       <c r="F24" s="7">
         <v>320.0</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="3">
         <v>1.0</v>
       </c>
       <c r="T24" s="7">
@@ -1540,29 +1602,29 @@
       <c r="V24" s="7">
         <v>2483.0</v>
       </c>
-      <c r="Y24" s="3"/>
+      <c r="Y24" s="1"/>
       <c r="Z24" s="5"/>
     </row>
     <row r="25">
-      <c r="A25" s="6" t="s">
-        <v>52</v>
+      <c r="A25" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B25" s="7">
         <v>303.28</v>
       </c>
-      <c r="C25" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D25" s="4">
+      <c r="C25" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="6">
         <v>204.38</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="3">
         <v>0.0</v>
       </c>
       <c r="F25" s="7">
         <v>335.71</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="3">
         <v>1.0</v>
       </c>
       <c r="T25" s="7">
@@ -1574,31 +1636,31 @@
       <c r="V25" s="7">
         <v>2419.0</v>
       </c>
-      <c r="Y25" s="3"/>
+      <c r="Y25" s="1"/>
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
       <c r="AB25" s="5"/>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="s">
-        <v>53</v>
+      <c r="A26" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="B26" s="7">
         <v>303.92</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="3">
         <v>1.0</v>
       </c>
       <c r="D26" s="7">
         <v>331.75</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="3">
         <v>1.0</v>
       </c>
       <c r="F26" s="7">
         <v>307.69</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="3">
         <v>1.0</v>
       </c>
       <c r="T26" s="7">
@@ -1612,25 +1674,25 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="s">
-        <v>54</v>
+      <c r="A27" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="B27" s="8">
         <v>247.19</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="3">
         <v>1.0</v>
       </c>
       <c r="D27" s="7">
         <v>277.11</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="3">
         <v>1.0</v>
       </c>
       <c r="F27" s="7">
         <v>271.6</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="3">
         <v>1.0</v>
       </c>
       <c r="T27" s="7">
@@ -1644,55 +1706,55 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="s">
-        <v>55</v>
+      <c r="A28" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B28" s="7">
         <v>310.34</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="3">
         <v>1.0</v>
       </c>
       <c r="D28" s="7">
         <v>327.49</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="3">
         <v>1.0</v>
       </c>
       <c r="F28" s="7">
         <v>328.77</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="3">
         <v>1.0</v>
       </c>
       <c r="H28" s="7">
         <v>331.13</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="3">
         <v>1.0</v>
       </c>
       <c r="J28" s="8">
         <v>262.5</v>
       </c>
-      <c r="K28" s="6">
+      <c r="K28" s="3">
         <v>1.0</v>
       </c>
       <c r="L28" s="8">
         <v>259.26</v>
       </c>
-      <c r="M28" s="6">
+      <c r="M28" s="3">
         <v>1.0</v>
       </c>
       <c r="N28" s="7">
         <v>301.2</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O28" s="3">
         <v>1.0</v>
       </c>
       <c r="P28" s="7">
         <v>301.2</v>
       </c>
-      <c r="Q28" s="6">
+      <c r="Q28" s="3">
         <v>1.0</v>
       </c>
       <c r="T28" s="5">
@@ -1706,25 +1768,25 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="4">
+      <c r="A29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="6">
         <v>370.08</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="3">
         <v>0.0</v>
       </c>
       <c r="D29" s="7">
         <v>407.69</v>
       </c>
-      <c r="E29" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F29" s="4">
+      <c r="E29" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F29" s="6">
         <v>488.37</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="3">
         <v>0.0</v>
       </c>
       <c r="T29" s="7">
@@ -1738,25 +1800,25 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="s">
-        <v>57</v>
+      <c r="A30" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="B30" s="7">
         <v>250.0</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="3">
         <v>1.0</v>
       </c>
       <c r="D30" s="7">
         <v>225.0</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="3">
         <v>1.0</v>
       </c>
       <c r="F30" s="7">
         <v>243.9</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="3">
         <v>1.0</v>
       </c>
       <c r="T30" s="7">
@@ -1770,25 +1832,25 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="s">
-        <v>58</v>
+      <c r="A31" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B31" s="7">
         <v>275.0</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="3">
         <v>1.0</v>
       </c>
       <c r="D31" s="7">
         <v>268.29</v>
       </c>
-      <c r="E31" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F31" s="6">
+      <c r="E31" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F31" s="3">
         <v>260.87</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="3">
         <v>1.0</v>
       </c>
       <c r="T31" s="7">
@@ -1802,25 +1864,25 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="s">
-        <v>59</v>
+      <c r="A32" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B32" s="7">
         <v>274.51</v>
       </c>
-      <c r="C32" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D32" s="4">
+      <c r="C32" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D32" s="6">
         <v>207.55</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="3">
         <v>0.0</v>
       </c>
       <c r="F32" s="7">
         <v>306.12</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="3">
         <v>1.0</v>
       </c>
       <c r="T32" s="7">
@@ -1834,31 +1896,31 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="s">
-        <v>60</v>
+      <c r="A33" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B33" s="7">
         <v>277.78</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="3">
         <v>1.0</v>
       </c>
       <c r="D33" s="7">
         <v>273.68</v>
       </c>
-      <c r="E33" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F33" s="4">
+      <c r="E33" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F33" s="6">
         <v>236.02</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="3">
         <v>0.0</v>
       </c>
       <c r="H33" s="7">
         <v>243.09</v>
       </c>
-      <c r="I33" s="6">
+      <c r="I33" s="3">
         <v>1.0</v>
       </c>
       <c r="T33" s="7">
@@ -1872,31 +1934,31 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="4">
+      <c r="A34" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="6">
         <v>276.32</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="3">
         <v>0.0</v>
       </c>
       <c r="D34" s="7">
         <v>318.47</v>
       </c>
-      <c r="E34" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F34" s="4">
+      <c r="E34" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F34" s="6">
         <v>251.66</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="3">
         <v>0.0</v>
       </c>
       <c r="H34" s="7">
         <v>324.68</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I34" s="3">
         <v>1.0</v>
       </c>
       <c r="T34" s="7">

</xml_diff>